<commit_message>
Trying to clean git repo
</commit_message>
<xml_diff>
--- a/data/zipcode_latlong.xlsx
+++ b/data/zipcode_latlong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdjor\OneDrive\Documents\Grad School Classes\SoftwareDesign\uwseds-group-transit-and-social-science\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="2AF6F34B7E39D78506CD6044EF51CB814C9A87D9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{B37D659F-C218-4A58-83DD-22B9DE7ED34A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="2AF6F34B7E39D78506CD6044EF51CB814C9A87D9" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{1A213E7B-A1E9-4052-86CE-44D1FEB6FAA0}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" xr2:uid="{5962265D-B6AD-4B78-89E2-0FDC0ADAD098}"/>
   </bookViews>
@@ -387,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93345042-18DC-43F1-B5B0-7C3A83590433}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -750,10 +750,10 @@
         <v>98195</v>
       </c>
       <c r="B33">
-        <v>47.651000000000003</v>
+        <v>47.65</v>
       </c>
       <c r="C33">
-        <v>-122.298</v>
+        <v>-122.31</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>